<commit_message>
implemented dbs and fixed cap file name
</commit_message>
<xml_diff>
--- a/docs/DBs.xlsx
+++ b/docs/DBs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Study\Project\old\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\osimseder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F29D4A-E794-4E26-BDF8-09E924511800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A71ED8C-706B-4EB3-B78F-9C505055B21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="2" activeTab="4" xr2:uid="{700CF38C-7C2E-434D-B0F8-DCB369BD3EE6}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="2" activeTab="4" xr2:uid="{700CF38C-7C2E-434D-B0F8-DCB369BD3EE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -59,24 +59,6 @@
     <t>PhoneNum</t>
   </si>
   <si>
-    <t>HouseID</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>taskID</t>
-  </si>
-  <si>
-    <t>House1</t>
-  </si>
-  <si>
-    <t>Houses-Tasks</t>
-  </si>
-  <si>
-    <t>taskType</t>
-  </si>
-  <si>
     <t>TaskType</t>
   </si>
   <si>
@@ -89,12 +71,6 @@
     <t>House Info</t>
   </si>
   <si>
-    <t>free text</t>
-  </si>
-  <si>
-    <t>Gear collection</t>
-  </si>
-  <si>
     <t>bathroom</t>
   </si>
   <si>
@@ -119,9 +95,6 @@
     <t>Staff</t>
   </si>
   <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
     <t>Last name</t>
   </si>
   <si>
@@ -161,30 +134,12 @@
     <t>STRING PK</t>
   </si>
   <si>
-    <t>hash</t>
-  </si>
-  <si>
     <t>STRING</t>
   </si>
   <si>
-    <t>ENUM</t>
-  </si>
-  <si>
     <t>STRING*</t>
   </si>
   <si>
-    <t>TEXT</t>
-  </si>
-  <si>
-    <t>ENUM*</t>
-  </si>
-  <si>
-    <t>Acesses</t>
-  </si>
-  <si>
-    <t>GroupID</t>
-  </si>
-  <si>
     <t>String PK</t>
   </si>
   <si>
@@ -194,9 +149,6 @@
     <t>IsInGroup(ID / -1)</t>
   </si>
   <si>
-    <t>GroupMembersIds ("ID1_ID2_ID3")</t>
-  </si>
-  <si>
     <t>String</t>
   </si>
   <si>
@@ -215,36 +167,9 @@
     <t>Schools</t>
   </si>
   <si>
-    <t>SchoolID</t>
-  </si>
-  <si>
-    <t>SchoolName</t>
-  </si>
-  <si>
-    <t>AreaID</t>
-  </si>
-  <si>
-    <t>AreaName</t>
-  </si>
-  <si>
-    <t>CityID</t>
-  </si>
-  <si>
-    <t>CityName</t>
-  </si>
-  <si>
     <t>String UNIQ</t>
   </si>
   <si>
-    <t>Resident Name</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>Need language assist? (ENUM/ null)</t>
-  </si>
-  <si>
     <t>Enum</t>
   </si>
   <si>
@@ -254,21 +179,9 @@
     <t>room</t>
   </si>
   <si>
-    <t>progress (1/2/3)</t>
-  </si>
-  <si>
-    <t>Picture-before</t>
-  </si>
-  <si>
-    <t>Picture-after</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
-    <t>House2</t>
-  </si>
-  <si>
     <t>painting</t>
   </si>
   <si>
@@ -293,25 +206,115 @@
     <t>Notes: Yello, paint, naylon, paint tools</t>
   </si>
   <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Extra info?</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
     <t>Any issues we should know about? (multiple choices: accessability, allergy, timing)</t>
   </si>
   <si>
-    <t>string_string_string</t>
-  </si>
-  <si>
-    <t>Tasks that needs proffesionals</t>
+    <t>INTEGER PK</t>
+  </si>
+  <si>
+    <t>STRING (hashed)</t>
+  </si>
+  <si>
+    <t>STRING (ENUM)</t>
+  </si>
+  <si>
+    <t>VerificationToken</t>
+  </si>
+  <si>
+    <t>STRING(ENUM) _ STRING (ENUM)</t>
+  </si>
+  <si>
+    <t>STRING (ENUM)_ STRING (ENUM)</t>
+  </si>
+  <si>
+    <t>languageNeeded</t>
+  </si>
+  <si>
+    <t>residentLastName</t>
+  </si>
+  <si>
+    <t>residentFirstName</t>
+  </si>
+  <si>
+    <t>residentPhoneNum</t>
+  </si>
+  <si>
+    <t>freeText</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>groupName</t>
+  </si>
+  <si>
+    <t>groupId</t>
+  </si>
+  <si>
+    <t>houseId</t>
+  </si>
+  <si>
+    <t>teamOwnerId</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>picAfter</t>
+  </si>
+  <si>
+    <t>picBefore</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>schoolName</t>
+  </si>
+  <si>
+    <t>areaId</t>
+  </si>
+  <si>
+    <t>cityId</t>
+  </si>
+  <si>
+    <t>Areas</t>
+  </si>
+  <si>
+    <t>areaName</t>
+  </si>
+  <si>
+    <t>Cities</t>
+  </si>
+  <si>
+    <t>cityName</t>
+  </si>
+  <si>
+    <t>accesses</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -471,13 +474,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -485,15 +488,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,7 +827,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -845,7 +839,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -859,9 +853,9 @@
       <selection sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -878,63 +872,63 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -952,7 +946,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -960,145 +954,149 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91312EE-ECAF-4746-A4FE-64E8FD662798}">
-  <dimension ref="B1:R1048562"/>
+  <dimension ref="A1:R1048551"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="4"/>
-    <col min="2" max="2" width="11.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="11.5546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="20" style="4" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="18" style="4" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11" style="4" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" style="4" customWidth="1"/>
     <col min="8" max="8" width="28" style="4" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="25.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="8.109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="27.109375" style="4" customWidth="1"/>
     <col min="14" max="14" width="24" style="4" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" style="4" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" style="4" customWidth="1"/>
     <col min="17" max="17" width="18" style="4" customWidth="1"/>
-    <col min="18" max="19" width="22.7109375" style="4" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" style="4" customWidth="1"/>
-    <col min="21" max="16384" width="8.85546875" style="4"/>
+    <col min="18" max="19" width="22.6640625" style="4" customWidth="1"/>
+    <col min="20" max="20" width="10.5546875" style="4" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="2:18" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="P2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="D3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="F3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="R2" s="17"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="K3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="R3" s="17"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R3" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1115,9 +1113,9 @@
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
-      <c r="R4" s="17"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R4" s="9"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1134,9 +1132,9 @@
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
-      <c r="R5" s="17"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="9"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1153,9 +1151,9 @@
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
-      <c r="R6" s="17"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="9"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1172,9 +1170,9 @@
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
-      <c r="R7" s="17"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R7" s="9"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1191,9 +1189,9 @@
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
-      <c r="R8" s="17"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R8" s="9"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1210,9 +1208,9 @@
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
-      <c r="R9" s="17"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R9" s="9"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -1229,9 +1227,9 @@
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
-      <c r="R10" s="17"/>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="9"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -1248,11 +1246,11 @@
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
-      <c r="R11" s="17"/>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R11" s="9"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="20" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
@@ -1267,9 +1265,9 @@
       <c r="M13" s="13"/>
       <c r="N13" s="14"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="20" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
@@ -1284,7 +1282,7 @@
       <c r="M14" s="13"/>
       <c r="N14" s="14"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
@@ -1299,85 +1297,79 @@
       <c r="M15" s="13"/>
       <c r="N15" s="14"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C16" s="11"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="K17" s="15"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>41</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="9"/>
       <c r="L18" s="16"/>
-      <c r="M18" s="23"/>
+      <c r="M18" s="12"/>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -1389,11 +1381,11 @@
       <c r="J19" s="6"/>
       <c r="K19" s="9"/>
       <c r="L19" s="16"/>
-      <c r="M19" s="23"/>
+      <c r="M19" s="12"/>
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -1405,11 +1397,11 @@
       <c r="J20" s="6"/>
       <c r="K20" s="9"/>
       <c r="L20" s="16"/>
-      <c r="M20" s="23"/>
+      <c r="M20" s="12"/>
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1421,11 +1413,11 @@
       <c r="J21" s="6"/>
       <c r="K21" s="9"/>
       <c r="L21" s="16"/>
-      <c r="M21" s="23"/>
+      <c r="M21" s="12"/>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1437,11 +1429,11 @@
       <c r="J22" s="6"/>
       <c r="K22" s="9"/>
       <c r="L22" s="16"/>
-      <c r="M22" s="23"/>
+      <c r="M22" s="12"/>
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -1453,11 +1445,11 @@
       <c r="J23" s="6"/>
       <c r="K23" s="9"/>
       <c r="L23" s="16"/>
-      <c r="M23" s="23"/>
+      <c r="M23" s="12"/>
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1469,11 +1461,11 @@
       <c r="J24" s="6"/>
       <c r="K24" s="9"/>
       <c r="L24" s="16"/>
-      <c r="M24" s="23"/>
+      <c r="M24" s="12"/>
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1485,11 +1477,11 @@
       <c r="J25" s="6"/>
       <c r="K25" s="9"/>
       <c r="L25" s="16"/>
-      <c r="M25" s="23"/>
+      <c r="M25" s="12"/>
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1501,79 +1493,95 @@
       <c r="J26" s="6"/>
       <c r="K26" s="9"/>
       <c r="L26" s="16"/>
-      <c r="M26" s="23"/>
+      <c r="M26" s="12"/>
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C30" s="11"/>
     </row>
-    <row r="31" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C40" s="6"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" s="21" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21"/>
@@ -1582,59 +1590,65 @@
       <c r="G42" s="21"/>
       <c r="H42" s="21"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C44" s="5"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="8" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="D45" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="F45" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="G45" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H45" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G45" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" s="6" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>85</v>
+        <v>35</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
@@ -1643,7 +1657,7 @@
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -1652,7 +1666,7 @@
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -1661,7 +1675,7 @@
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
@@ -1670,7 +1684,7 @@
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
@@ -1679,7 +1693,7 @@
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -1688,7 +1702,7 @@
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -1697,7 +1711,7 @@
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -1706,74 +1720,78 @@
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="I58" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J58" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K58" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J58" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B59" s="6" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="K59" s="7"/>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B60" s="8">
         <v>1</v>
       </c>
@@ -1781,22 +1799,23 @@
         <v>1</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F60" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K60" s="7"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B61" s="8">
         <v>2</v>
       </c>
@@ -1804,18 +1823,19 @@
         <v>2</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="8" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K61" s="7"/>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B62" s="8">
         <v>3</v>
       </c>
@@ -1823,18 +1843,19 @@
         <v>3</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K62" s="7"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
@@ -1844,8 +1865,9 @@
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K63" s="7"/>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
@@ -1855,8 +1877,9 @@
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K64" s="7"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -1866,8 +1889,9 @@
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K65" s="7"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
@@ -1877,8 +1901,9 @@
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K66" s="7"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -1888,273 +1913,295 @@
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" s="5"/>
-      <c r="C69" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" s="10" t="s">
+      <c r="K67" s="7"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B71" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C72" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C72" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B73" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B74" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="7"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B75" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C75" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B76" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C76" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="7"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="7"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B83" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B84" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C84" s="8" t="s">
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="7"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="7"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B84" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D84" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="7"/>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>81</v>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B85" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B86" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
       <c r="D87" s="7"/>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E87" s="8"/>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B88" s="8"/>
-      <c r="C88" s="8"/>
+      <c r="C88" s="7"/>
       <c r="D88" s="7"/>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E88" s="8"/>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
       <c r="D89" s="7"/>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E89" s="8"/>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
       <c r="D90" s="7"/>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E90" s="8"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
       <c r="D91" s="7"/>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E91" s="8"/>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
       <c r="D92" s="7"/>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G96" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F97" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G97" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="8"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="7"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="7"/>
-      <c r="G98" s="7"/>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="8"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="7"/>
-      <c r="E99" s="8"/>
-      <c r="F99" s="7"/>
-      <c r="G99" s="7"/>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E92" s="8"/>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="8"/>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="8"/>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B97" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B98" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B99" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
       <c r="D100" s="7"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="7"/>
-      <c r="G100" s="7"/>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B101" s="8"/>
-      <c r="C101" s="8"/>
+      <c r="C101" s="7"/>
       <c r="D101" s="7"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="7"/>
-      <c r="G101" s="7"/>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
       <c r="D102" s="7"/>
-      <c r="E102" s="8"/>
-      <c r="F102" s="7"/>
-      <c r="G102" s="7"/>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
       <c r="D103" s="7"/>
-      <c r="E103" s="8"/>
-      <c r="F103" s="7"/>
-      <c r="G103" s="7"/>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
       <c r="D104" s="7"/>
-      <c r="E104" s="8"/>
-      <c r="F104" s="7"/>
-      <c r="G104" s="7"/>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
       <c r="D105" s="7"/>
-      <c r="E105" s="8"/>
-      <c r="F105" s="7"/>
-      <c r="G105" s="7"/>
-    </row>
-    <row r="1048562" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1048562" s="8"/>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="7"/>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B107" s="8"/>
+      <c r="C107" s="8"/>
+      <c r="D107" s="7"/>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B110" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B111" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B112" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B114" s="8"/>
+      <c r="C114" s="7"/>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B115" s="8"/>
+      <c r="C115" s="8"/>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B116" s="8"/>
+      <c r="C116" s="8"/>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B117" s="8"/>
+      <c r="C117" s="8"/>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B119" s="8"/>
+      <c r="C119" s="8"/>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
+    </row>
+    <row r="1048551" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F1048551" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2173,7 +2220,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2185,7 +2232,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>